<commit_message>
Updates to the script to create draft of the resourceRelationship, eMOF and occurrence extensions.
</commit_message>
<xml_diff>
--- a/IYS_data_template/IYS2022_NW_Data_v1.xlsx
+++ b/IYS_data_template/IYS2022_NW_Data_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\GitHub\2022-NW-Trawl\IYS_data_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C270F49A-9A2B-4EDD-99C0-F76C62A2A793}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A729E60E-1536-43FC-BEB1-BF4BC6EC19C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -6165,8 +6165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A977" workbookViewId="0">
+      <selection activeCell="H997" sqref="H997"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6176,7 +6176,8 @@
     <col min="3" max="3" width="30.21875" customWidth="1"/>
     <col min="4" max="4" width="25.109375" customWidth="1"/>
     <col min="5" max="5" width="27.109375" customWidth="1"/>
-    <col min="6" max="8" width="10.21875" customWidth="1"/>
+    <col min="6" max="7" width="10.21875" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
     <col min="10" max="11" width="8.77734375" customWidth="1"/>
     <col min="12" max="240" width="8.6640625" customWidth="1"/>
@@ -49265,8 +49266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="L148" sqref="L148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>